<commit_message>
new plots and descriptions
</commit_message>
<xml_diff>
--- a/FilteredInput/cleaned_yield_data.xlsx
+++ b/FilteredInput/cleaned_yield_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H159"/>
+  <dimension ref="A1:M159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,32 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>strip</t>
+          <t>mean_temp_year</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>total_rainfall_year</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>total_Metopolophium dirhodum</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>total_Rhopalosiphum padi</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>total_Sitobion avenae</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>CO2e_total_kg</t>
         </is>
       </c>
     </row>
@@ -504,7 +529,22 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I2" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J2" t="n">
+        <v>579</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L2" t="n">
+        <v>324</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="3">
@@ -536,7 +576,22 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I3" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>579</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L3" t="n">
+        <v>324</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="4">
@@ -568,7 +623,22 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I4" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J4" t="n">
+        <v>579</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L4" t="n">
+        <v>324</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="5">
@@ -600,7 +670,22 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I5" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J5" t="n">
+        <v>579</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L5" t="n">
+        <v>324</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +717,22 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I6" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J6" t="n">
+        <v>579</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L6" t="n">
+        <v>324</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="7">
@@ -664,7 +764,22 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I7" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J7" t="n">
+        <v>579</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L7" t="n">
+        <v>324</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="8">
@@ -696,7 +811,22 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I8" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J8" t="n">
+        <v>579</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L8" t="n">
+        <v>324</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="9">
@@ -728,7 +858,22 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>8</v>
+        <v>10.4713470515</v>
+      </c>
+      <c r="I9" t="n">
+        <v>709.0035599999999</v>
+      </c>
+      <c r="J9" t="n">
+        <v>579</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1256</v>
+      </c>
+      <c r="L9" t="n">
+        <v>324</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="10">
@@ -760,7 +905,22 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I10" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J10" t="n">
+        <v>415</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="11">
@@ -792,7 +952,22 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I11" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J11" t="n">
+        <v>415</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="12">
@@ -824,7 +999,22 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I12" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J12" t="n">
+        <v>415</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="13">
@@ -856,7 +1046,22 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I13" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J13" t="n">
+        <v>415</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="14">
@@ -888,7 +1093,22 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I14" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J14" t="n">
+        <v>415</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="15">
@@ -920,7 +1140,22 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I15" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J15" t="n">
+        <v>415</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="16">
@@ -952,7 +1187,22 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I16" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J16" t="n">
+        <v>415</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="17">
@@ -984,7 +1234,22 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>8</v>
+        <v>9.14304609925</v>
+      </c>
+      <c r="I17" t="n">
+        <v>776.3224200000001</v>
+      </c>
+      <c r="J17" t="n">
+        <v>415</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2683</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="18">
@@ -1016,7 +1281,22 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I18" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K18" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L18" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="19">
@@ -1048,7 +1328,22 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I19" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J19" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K19" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L19" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="20">
@@ -1080,7 +1375,22 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I20" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J20" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L20" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="21">
@@ -1112,7 +1422,22 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I21" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K21" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L21" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="22">
@@ -1144,7 +1469,22 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I22" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J22" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K22" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L22" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="23">
@@ -1176,7 +1516,22 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I23" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J23" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K23" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L23" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="24">
@@ -1208,7 +1563,22 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I24" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J24" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K24" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L24" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="25">
@@ -1240,7 +1610,22 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>8</v>
+        <v>10.002850274</v>
+      </c>
+      <c r="I25" t="n">
+        <v>714.42002</v>
+      </c>
+      <c r="J25" t="n">
+        <v>4775</v>
+      </c>
+      <c r="K25" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L25" t="n">
+        <v>4911</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="26">
@@ -1272,7 +1657,22 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I26" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J26" t="n">
+        <v>381</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L26" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="27">
@@ -1304,7 +1704,22 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I27" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J27" t="n">
+        <v>381</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L27" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="28">
@@ -1336,7 +1751,22 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I28" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J28" t="n">
+        <v>381</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L28" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M28" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="29">
@@ -1368,7 +1798,22 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I29" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J29" t="n">
+        <v>381</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M29" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="30">
@@ -1400,7 +1845,22 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I30" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J30" t="n">
+        <v>381</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="31">
@@ -1432,7 +1892,22 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I31" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J31" t="n">
+        <v>381</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="32">
@@ -1464,7 +1939,22 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I32" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J32" t="n">
+        <v>381</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L32" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="33">
@@ -1496,7 +1986,22 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>8</v>
+        <v>9.48823883725</v>
+      </c>
+      <c r="I33" t="n">
+        <v>935.7211</v>
+      </c>
+      <c r="J33" t="n">
+        <v>381</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1349</v>
+      </c>
+      <c r="L33" t="n">
+        <v>2123</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="34">
@@ -1528,7 +2033,22 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I34" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K34" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L34" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="35">
@@ -1560,7 +2080,22 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I35" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K35" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L35" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="36">
@@ -1592,7 +2127,22 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I36" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J36" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K36" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L36" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="37">
@@ -1624,7 +2174,22 @@
         </is>
       </c>
       <c r="H37" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I37" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J37" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K37" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L37" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="38">
@@ -1656,7 +2221,22 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I38" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J38" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K38" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L38" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M38" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="39">
@@ -1688,7 +2268,22 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I39" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J39" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K39" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L39" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="40">
@@ -1720,7 +2315,22 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>8</v>
+        <v>9.5933518805</v>
+      </c>
+      <c r="I40" t="n">
+        <v>934.50516</v>
+      </c>
+      <c r="J40" t="n">
+        <v>2583</v>
+      </c>
+      <c r="K40" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L40" t="n">
+        <v>6747</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="41">
@@ -1752,7 +2362,22 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I41" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J41" t="n">
+        <v>229</v>
+      </c>
+      <c r="K41" t="n">
+        <v>820</v>
+      </c>
+      <c r="L41" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M41" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="42">
@@ -1784,7 +2409,22 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I42" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J42" t="n">
+        <v>229</v>
+      </c>
+      <c r="K42" t="n">
+        <v>820</v>
+      </c>
+      <c r="L42" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M42" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="43">
@@ -1816,7 +2456,22 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I43" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J43" t="n">
+        <v>229</v>
+      </c>
+      <c r="K43" t="n">
+        <v>820</v>
+      </c>
+      <c r="L43" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M43" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="44">
@@ -1848,7 +2503,22 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I44" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J44" t="n">
+        <v>229</v>
+      </c>
+      <c r="K44" t="n">
+        <v>820</v>
+      </c>
+      <c r="L44" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M44" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="45">
@@ -1880,7 +2550,22 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I45" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J45" t="n">
+        <v>229</v>
+      </c>
+      <c r="K45" t="n">
+        <v>820</v>
+      </c>
+      <c r="L45" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M45" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="46">
@@ -1912,7 +2597,22 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I46" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J46" t="n">
+        <v>229</v>
+      </c>
+      <c r="K46" t="n">
+        <v>820</v>
+      </c>
+      <c r="L46" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M46" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="47">
@@ -1944,7 +2644,22 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I47" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J47" t="n">
+        <v>229</v>
+      </c>
+      <c r="K47" t="n">
+        <v>820</v>
+      </c>
+      <c r="L47" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M47" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="48">
@@ -1976,7 +2691,22 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>8</v>
+        <v>10.57316965825</v>
+      </c>
+      <c r="I48" t="n">
+        <v>706.9033000000002</v>
+      </c>
+      <c r="J48" t="n">
+        <v>229</v>
+      </c>
+      <c r="K48" t="n">
+        <v>820</v>
+      </c>
+      <c r="L48" t="n">
+        <v>3983</v>
+      </c>
+      <c r="M48" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="49">
@@ -2008,7 +2738,22 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I49" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J49" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K49" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L49" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M49" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="50">
@@ -2040,7 +2785,22 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I50" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K50" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L50" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M50" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="51">
@@ -2072,7 +2832,22 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I51" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J51" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K51" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L51" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M51" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="52">
@@ -2104,7 +2879,22 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I52" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K52" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L52" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M52" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="53">
@@ -2136,7 +2926,22 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I53" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K53" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L53" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M53" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="54">
@@ -2168,7 +2973,22 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I54" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K54" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L54" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M54" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="55">
@@ -2200,7 +3020,22 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I55" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K55" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L55" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M55" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="56">
@@ -2232,7 +3067,22 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>8</v>
+        <v>9.243593227250001</v>
+      </c>
+      <c r="I56" t="n">
+        <v>652.7387</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1101</v>
+      </c>
+      <c r="K56" t="n">
+        <v>2169</v>
+      </c>
+      <c r="L56" t="n">
+        <v>12803</v>
+      </c>
+      <c r="M56" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="57">
@@ -2264,7 +3114,22 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I57" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J57" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K57" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L57" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M57" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="58">
@@ -2296,7 +3161,22 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I58" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J58" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K58" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L58" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M58" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="59">
@@ -2328,7 +3208,22 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I59" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J59" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K59" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L59" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M59" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="60">
@@ -2360,7 +3255,22 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I60" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J60" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K60" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L60" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M60" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="61">
@@ -2392,7 +3302,22 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I61" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J61" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K61" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L61" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M61" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="62">
@@ -2424,7 +3349,22 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I62" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J62" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K62" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L62" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M62" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="63">
@@ -2456,7 +3396,22 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I63" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J63" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K63" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L63" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M63" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="64">
@@ -2488,7 +3443,22 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>8</v>
+        <v>9.92623058975</v>
+      </c>
+      <c r="I64" t="n">
+        <v>633.1731199999999</v>
+      </c>
+      <c r="J64" t="n">
+        <v>5640</v>
+      </c>
+      <c r="K64" t="n">
+        <v>4720</v>
+      </c>
+      <c r="L64" t="n">
+        <v>2247</v>
+      </c>
+      <c r="M64" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="65">
@@ -2520,7 +3490,22 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I65" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J65" t="n">
+        <v>41</v>
+      </c>
+      <c r="K65" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L65" t="n">
+        <v>385</v>
+      </c>
+      <c r="M65" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="66">
@@ -2552,7 +3537,22 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I66" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J66" t="n">
+        <v>41</v>
+      </c>
+      <c r="K66" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L66" t="n">
+        <v>385</v>
+      </c>
+      <c r="M66" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="67">
@@ -2584,7 +3584,22 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I67" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J67" t="n">
+        <v>41</v>
+      </c>
+      <c r="K67" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L67" t="n">
+        <v>385</v>
+      </c>
+      <c r="M67" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="68">
@@ -2616,7 +3631,22 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I68" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J68" t="n">
+        <v>41</v>
+      </c>
+      <c r="K68" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L68" t="n">
+        <v>385</v>
+      </c>
+      <c r="M68" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="69">
@@ -2648,7 +3678,22 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I69" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J69" t="n">
+        <v>41</v>
+      </c>
+      <c r="K69" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L69" t="n">
+        <v>385</v>
+      </c>
+      <c r="M69" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="70">
@@ -2680,7 +3725,22 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I70" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J70" t="n">
+        <v>41</v>
+      </c>
+      <c r="K70" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L70" t="n">
+        <v>385</v>
+      </c>
+      <c r="M70" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="71">
@@ -2712,7 +3772,22 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I71" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J71" t="n">
+        <v>41</v>
+      </c>
+      <c r="K71" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L71" t="n">
+        <v>385</v>
+      </c>
+      <c r="M71" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="72">
@@ -2744,7 +3819,22 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>8</v>
+        <v>10.25889257125</v>
+      </c>
+      <c r="I72" t="n">
+        <v>726.35834</v>
+      </c>
+      <c r="J72" t="n">
+        <v>41</v>
+      </c>
+      <c r="K72" t="n">
+        <v>1374</v>
+      </c>
+      <c r="L72" t="n">
+        <v>385</v>
+      </c>
+      <c r="M72" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="73">
@@ -2776,7 +3866,22 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I73" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J73" t="n">
+        <v>265</v>
+      </c>
+      <c r="K73" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L73" t="n">
+        <v>920</v>
+      </c>
+      <c r="M73" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="74">
@@ -2808,7 +3913,22 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I74" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J74" t="n">
+        <v>265</v>
+      </c>
+      <c r="K74" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L74" t="n">
+        <v>920</v>
+      </c>
+      <c r="M74" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="75">
@@ -2840,7 +3960,22 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I75" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J75" t="n">
+        <v>265</v>
+      </c>
+      <c r="K75" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L75" t="n">
+        <v>920</v>
+      </c>
+      <c r="M75" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="76">
@@ -2872,7 +4007,22 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I76" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J76" t="n">
+        <v>265</v>
+      </c>
+      <c r="K76" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L76" t="n">
+        <v>920</v>
+      </c>
+      <c r="M76" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="77">
@@ -2904,7 +4054,22 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I77" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J77" t="n">
+        <v>265</v>
+      </c>
+      <c r="K77" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L77" t="n">
+        <v>920</v>
+      </c>
+      <c r="M77" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="78">
@@ -2936,7 +4101,22 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I78" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J78" t="n">
+        <v>265</v>
+      </c>
+      <c r="K78" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L78" t="n">
+        <v>920</v>
+      </c>
+      <c r="M78" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="79">
@@ -2968,7 +4148,22 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I79" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J79" t="n">
+        <v>265</v>
+      </c>
+      <c r="K79" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L79" t="n">
+        <v>920</v>
+      </c>
+      <c r="M79" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="80">
@@ -3000,7 +4195,22 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>8</v>
+        <v>10.29818976425</v>
+      </c>
+      <c r="I80" t="n">
+        <v>951.63886</v>
+      </c>
+      <c r="J80" t="n">
+        <v>265</v>
+      </c>
+      <c r="K80" t="n">
+        <v>1757</v>
+      </c>
+      <c r="L80" t="n">
+        <v>920</v>
+      </c>
+      <c r="M80" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="81">
@@ -3032,7 +4242,22 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I81" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J81" t="n">
+        <v>75</v>
+      </c>
+      <c r="K81" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L81" t="n">
+        <v>877</v>
+      </c>
+      <c r="M81" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="82">
@@ -3064,7 +4289,22 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I82" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J82" t="n">
+        <v>75</v>
+      </c>
+      <c r="K82" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L82" t="n">
+        <v>877</v>
+      </c>
+      <c r="M82" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="83">
@@ -3096,7 +4336,22 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I83" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J83" t="n">
+        <v>75</v>
+      </c>
+      <c r="K83" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L83" t="n">
+        <v>877</v>
+      </c>
+      <c r="M83" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="84">
@@ -3128,7 +4383,22 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I84" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J84" t="n">
+        <v>75</v>
+      </c>
+      <c r="K84" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L84" t="n">
+        <v>877</v>
+      </c>
+      <c r="M84" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="85">
@@ -3160,7 +4430,22 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I85" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J85" t="n">
+        <v>75</v>
+      </c>
+      <c r="K85" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L85" t="n">
+        <v>877</v>
+      </c>
+      <c r="M85" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="86">
@@ -3192,7 +4477,22 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I86" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J86" t="n">
+        <v>75</v>
+      </c>
+      <c r="K86" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L86" t="n">
+        <v>877</v>
+      </c>
+      <c r="M86" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="87">
@@ -3224,7 +4524,22 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I87" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J87" t="n">
+        <v>75</v>
+      </c>
+      <c r="K87" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L87" t="n">
+        <v>877</v>
+      </c>
+      <c r="M87" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="88">
@@ -3256,7 +4571,22 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>8</v>
+        <v>10.263630256</v>
+      </c>
+      <c r="I88" t="n">
+        <v>794.0088199999999</v>
+      </c>
+      <c r="J88" t="n">
+        <v>75</v>
+      </c>
+      <c r="K88" t="n">
+        <v>1351</v>
+      </c>
+      <c r="L88" t="n">
+        <v>877</v>
+      </c>
+      <c r="M88" t="n">
+        <v>1699.532</v>
       </c>
     </row>
     <row r="89">
@@ -3288,7 +4618,22 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I89" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J89" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K89" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L89" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M89" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="90">
@@ -3320,7 +4665,22 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I90" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J90" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K90" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L90" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M90" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="91">
@@ -3352,7 +4712,22 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I91" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J91" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K91" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L91" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M91" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="92">
@@ -3384,7 +4759,22 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I92" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J92" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K92" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L92" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M92" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="93">
@@ -3416,7 +4806,22 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I93" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J93" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K93" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L93" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M93" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="94">
@@ -3448,7 +4853,22 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I94" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J94" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K94" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L94" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M94" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="95">
@@ -3480,7 +4900,22 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I95" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J95" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K95" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L95" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M95" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="96">
@@ -3512,7 +4947,22 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>8</v>
+        <v>9.70129622</v>
+      </c>
+      <c r="I96" t="n">
+        <v>717.3</v>
+      </c>
+      <c r="J96" t="n">
+        <v>2448</v>
+      </c>
+      <c r="K96" t="n">
+        <v>2040</v>
+      </c>
+      <c r="L96" t="n">
+        <v>2382</v>
+      </c>
+      <c r="M96" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="97">
@@ -3544,7 +4994,22 @@
         </is>
       </c>
       <c r="H97" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I97" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J97" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K97" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L97" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M97" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="98">
@@ -3576,7 +5041,22 @@
         </is>
       </c>
       <c r="H98" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I98" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J98" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K98" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L98" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M98" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="99">
@@ -3608,7 +5088,22 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I99" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J99" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K99" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L99" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M99" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="100">
@@ -3640,7 +5135,22 @@
         </is>
       </c>
       <c r="H100" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I100" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J100" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K100" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L100" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M100" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="101">
@@ -3672,7 +5182,22 @@
         </is>
       </c>
       <c r="H101" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I101" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J101" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K101" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L101" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M101" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="102">
@@ -3704,7 +5229,22 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I102" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J102" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K102" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L102" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M102" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="103">
@@ -3736,7 +5276,22 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I103" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J103" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K103" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L103" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M103" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="104">
@@ -3768,7 +5323,22 @@
         </is>
       </c>
       <c r="H104" t="n">
-        <v>8</v>
+        <v>9.629243245750001</v>
+      </c>
+      <c r="I104" t="n">
+        <v>623.7</v>
+      </c>
+      <c r="J104" t="n">
+        <v>2519</v>
+      </c>
+      <c r="K104" t="n">
+        <v>4968</v>
+      </c>
+      <c r="L104" t="n">
+        <v>5991</v>
+      </c>
+      <c r="M104" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="105">
@@ -3800,7 +5370,22 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I105" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J105" t="n">
+        <v>86</v>
+      </c>
+      <c r="K105" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L105" t="n">
+        <v>434</v>
+      </c>
+      <c r="M105" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="106">
@@ -3832,7 +5417,22 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I106" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J106" t="n">
+        <v>86</v>
+      </c>
+      <c r="K106" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L106" t="n">
+        <v>434</v>
+      </c>
+      <c r="M106" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="107">
@@ -3864,7 +5464,22 @@
         </is>
       </c>
       <c r="H107" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I107" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J107" t="n">
+        <v>86</v>
+      </c>
+      <c r="K107" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L107" t="n">
+        <v>434</v>
+      </c>
+      <c r="M107" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="108">
@@ -3896,7 +5511,22 @@
         </is>
       </c>
       <c r="H108" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I108" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J108" t="n">
+        <v>86</v>
+      </c>
+      <c r="K108" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L108" t="n">
+        <v>434</v>
+      </c>
+      <c r="M108" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="109">
@@ -3928,7 +5558,22 @@
         </is>
       </c>
       <c r="H109" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I109" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J109" t="n">
+        <v>86</v>
+      </c>
+      <c r="K109" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L109" t="n">
+        <v>434</v>
+      </c>
+      <c r="M109" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="110">
@@ -3960,7 +5605,22 @@
         </is>
       </c>
       <c r="H110" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I110" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J110" t="n">
+        <v>86</v>
+      </c>
+      <c r="K110" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L110" t="n">
+        <v>434</v>
+      </c>
+      <c r="M110" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="111">
@@ -3992,7 +5652,22 @@
         </is>
       </c>
       <c r="H111" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I111" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J111" t="n">
+        <v>86</v>
+      </c>
+      <c r="K111" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L111" t="n">
+        <v>434</v>
+      </c>
+      <c r="M111" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="112">
@@ -4024,7 +5699,22 @@
         </is>
       </c>
       <c r="H112" t="n">
-        <v>8</v>
+        <v>10.525347886</v>
+      </c>
+      <c r="I112" t="n">
+        <v>870.8</v>
+      </c>
+      <c r="J112" t="n">
+        <v>86</v>
+      </c>
+      <c r="K112" t="n">
+        <v>1833</v>
+      </c>
+      <c r="L112" t="n">
+        <v>434</v>
+      </c>
+      <c r="M112" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="113">
@@ -4056,7 +5746,22 @@
         </is>
       </c>
       <c r="H113" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I113" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J113" t="n">
+        <v>151</v>
+      </c>
+      <c r="K113" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L113" t="n">
+        <v>437</v>
+      </c>
+      <c r="M113" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="114">
@@ -4088,7 +5793,22 @@
         </is>
       </c>
       <c r="H114" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I114" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J114" t="n">
+        <v>151</v>
+      </c>
+      <c r="K114" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L114" t="n">
+        <v>437</v>
+      </c>
+      <c r="M114" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="115">
@@ -4120,7 +5840,22 @@
         </is>
       </c>
       <c r="H115" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I115" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J115" t="n">
+        <v>151</v>
+      </c>
+      <c r="K115" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L115" t="n">
+        <v>437</v>
+      </c>
+      <c r="M115" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="116">
@@ -4152,7 +5887,22 @@
         </is>
       </c>
       <c r="H116" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I116" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J116" t="n">
+        <v>151</v>
+      </c>
+      <c r="K116" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L116" t="n">
+        <v>437</v>
+      </c>
+      <c r="M116" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="117">
@@ -4184,7 +5934,22 @@
         </is>
       </c>
       <c r="H117" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I117" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J117" t="n">
+        <v>151</v>
+      </c>
+      <c r="K117" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L117" t="n">
+        <v>437</v>
+      </c>
+      <c r="M117" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="118">
@@ -4216,7 +5981,22 @@
         </is>
       </c>
       <c r="H118" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I118" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J118" t="n">
+        <v>151</v>
+      </c>
+      <c r="K118" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L118" t="n">
+        <v>437</v>
+      </c>
+      <c r="M118" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="119">
@@ -4248,7 +6028,22 @@
         </is>
       </c>
       <c r="H119" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I119" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J119" t="n">
+        <v>151</v>
+      </c>
+      <c r="K119" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L119" t="n">
+        <v>437</v>
+      </c>
+      <c r="M119" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="120">
@@ -4280,7 +6075,22 @@
         </is>
       </c>
       <c r="H120" t="n">
-        <v>8</v>
+        <v>9.14851651625</v>
+      </c>
+      <c r="I120" t="n">
+        <v>778.3000000000001</v>
+      </c>
+      <c r="J120" t="n">
+        <v>151</v>
+      </c>
+      <c r="K120" t="n">
+        <v>1081</v>
+      </c>
+      <c r="L120" t="n">
+        <v>437</v>
+      </c>
+      <c r="M120" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="121">
@@ -4312,7 +6122,22 @@
         </is>
       </c>
       <c r="H121" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I121" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J121" t="n">
+        <v>150</v>
+      </c>
+      <c r="K121" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L121" t="n">
+        <v>384</v>
+      </c>
+      <c r="M121" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="122">
@@ -4344,7 +6169,22 @@
         </is>
       </c>
       <c r="H122" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I122" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J122" t="n">
+        <v>150</v>
+      </c>
+      <c r="K122" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L122" t="n">
+        <v>384</v>
+      </c>
+      <c r="M122" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="123">
@@ -4376,7 +6216,22 @@
         </is>
       </c>
       <c r="H123" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I123" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J123" t="n">
+        <v>150</v>
+      </c>
+      <c r="K123" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L123" t="n">
+        <v>384</v>
+      </c>
+      <c r="M123" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="124">
@@ -4408,7 +6263,22 @@
         </is>
       </c>
       <c r="H124" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I124" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J124" t="n">
+        <v>150</v>
+      </c>
+      <c r="K124" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L124" t="n">
+        <v>384</v>
+      </c>
+      <c r="M124" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="125">
@@ -4440,7 +6310,22 @@
         </is>
       </c>
       <c r="H125" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I125" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J125" t="n">
+        <v>150</v>
+      </c>
+      <c r="K125" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L125" t="n">
+        <v>384</v>
+      </c>
+      <c r="M125" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="126">
@@ -4472,7 +6357,22 @@
         </is>
       </c>
       <c r="H126" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I126" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J126" t="n">
+        <v>150</v>
+      </c>
+      <c r="K126" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L126" t="n">
+        <v>384</v>
+      </c>
+      <c r="M126" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="127">
@@ -4504,7 +6404,22 @@
         </is>
       </c>
       <c r="H127" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I127" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J127" t="n">
+        <v>150</v>
+      </c>
+      <c r="K127" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L127" t="n">
+        <v>384</v>
+      </c>
+      <c r="M127" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="128">
@@ -4536,7 +6451,22 @@
         </is>
       </c>
       <c r="H128" t="n">
-        <v>8</v>
+        <v>10.87966458975</v>
+      </c>
+      <c r="I128" t="n">
+        <v>982.9</v>
+      </c>
+      <c r="J128" t="n">
+        <v>150</v>
+      </c>
+      <c r="K128" t="n">
+        <v>4315</v>
+      </c>
+      <c r="L128" t="n">
+        <v>384</v>
+      </c>
+      <c r="M128" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="129">
@@ -4568,7 +6498,22 @@
         </is>
       </c>
       <c r="H129" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I129" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J129" t="n">
+        <v>110</v>
+      </c>
+      <c r="K129" t="n">
+        <v>927</v>
+      </c>
+      <c r="L129" t="n">
+        <v>111</v>
+      </c>
+      <c r="M129" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="130">
@@ -4600,7 +6545,22 @@
         </is>
       </c>
       <c r="H130" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I130" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J130" t="n">
+        <v>110</v>
+      </c>
+      <c r="K130" t="n">
+        <v>927</v>
+      </c>
+      <c r="L130" t="n">
+        <v>111</v>
+      </c>
+      <c r="M130" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="131">
@@ -4632,7 +6592,22 @@
         </is>
       </c>
       <c r="H131" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I131" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J131" t="n">
+        <v>110</v>
+      </c>
+      <c r="K131" t="n">
+        <v>927</v>
+      </c>
+      <c r="L131" t="n">
+        <v>111</v>
+      </c>
+      <c r="M131" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="132">
@@ -4664,7 +6639,22 @@
         </is>
       </c>
       <c r="H132" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I132" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J132" t="n">
+        <v>110</v>
+      </c>
+      <c r="K132" t="n">
+        <v>927</v>
+      </c>
+      <c r="L132" t="n">
+        <v>111</v>
+      </c>
+      <c r="M132" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="133">
@@ -4696,7 +6686,22 @@
         </is>
       </c>
       <c r="H133" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I133" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J133" t="n">
+        <v>110</v>
+      </c>
+      <c r="K133" t="n">
+        <v>927</v>
+      </c>
+      <c r="L133" t="n">
+        <v>111</v>
+      </c>
+      <c r="M133" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="134">
@@ -4728,7 +6733,22 @@
         </is>
       </c>
       <c r="H134" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I134" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J134" t="n">
+        <v>110</v>
+      </c>
+      <c r="K134" t="n">
+        <v>927</v>
+      </c>
+      <c r="L134" t="n">
+        <v>111</v>
+      </c>
+      <c r="M134" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="135">
@@ -4760,7 +6780,22 @@
         </is>
       </c>
       <c r="H135" t="n">
-        <v>8</v>
+        <v>10.7708836005</v>
+      </c>
+      <c r="I135" t="n">
+        <v>742.8</v>
+      </c>
+      <c r="J135" t="n">
+        <v>110</v>
+      </c>
+      <c r="K135" t="n">
+        <v>927</v>
+      </c>
+      <c r="L135" t="n">
+        <v>111</v>
+      </c>
+      <c r="M135" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="136">
@@ -4792,7 +6827,22 @@
         </is>
       </c>
       <c r="H136" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I136" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J136" t="n">
+        <v>91</v>
+      </c>
+      <c r="K136" t="n">
+        <v>660</v>
+      </c>
+      <c r="L136" t="n">
+        <v>106</v>
+      </c>
+      <c r="M136" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="137">
@@ -4824,7 +6874,22 @@
         </is>
       </c>
       <c r="H137" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I137" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J137" t="n">
+        <v>91</v>
+      </c>
+      <c r="K137" t="n">
+        <v>660</v>
+      </c>
+      <c r="L137" t="n">
+        <v>106</v>
+      </c>
+      <c r="M137" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="138">
@@ -4856,7 +6921,22 @@
         </is>
       </c>
       <c r="H138" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I138" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J138" t="n">
+        <v>91</v>
+      </c>
+      <c r="K138" t="n">
+        <v>660</v>
+      </c>
+      <c r="L138" t="n">
+        <v>106</v>
+      </c>
+      <c r="M138" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="139">
@@ -4888,7 +6968,22 @@
         </is>
       </c>
       <c r="H139" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I139" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J139" t="n">
+        <v>91</v>
+      </c>
+      <c r="K139" t="n">
+        <v>660</v>
+      </c>
+      <c r="L139" t="n">
+        <v>106</v>
+      </c>
+      <c r="M139" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="140">
@@ -4920,7 +7015,22 @@
         </is>
       </c>
       <c r="H140" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I140" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J140" t="n">
+        <v>91</v>
+      </c>
+      <c r="K140" t="n">
+        <v>660</v>
+      </c>
+      <c r="L140" t="n">
+        <v>106</v>
+      </c>
+      <c r="M140" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="141">
@@ -4952,7 +7062,22 @@
         </is>
       </c>
       <c r="H141" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I141" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J141" t="n">
+        <v>91</v>
+      </c>
+      <c r="K141" t="n">
+        <v>660</v>
+      </c>
+      <c r="L141" t="n">
+        <v>106</v>
+      </c>
+      <c r="M141" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="142">
@@ -4984,7 +7109,22 @@
         </is>
       </c>
       <c r="H142" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I142" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J142" t="n">
+        <v>91</v>
+      </c>
+      <c r="K142" t="n">
+        <v>660</v>
+      </c>
+      <c r="L142" t="n">
+        <v>106</v>
+      </c>
+      <c r="M142" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="143">
@@ -5016,7 +7156,22 @@
         </is>
       </c>
       <c r="H143" t="n">
-        <v>8</v>
+        <v>10.6930498805</v>
+      </c>
+      <c r="I143" t="n">
+        <v>622.2</v>
+      </c>
+      <c r="J143" t="n">
+        <v>91</v>
+      </c>
+      <c r="K143" t="n">
+        <v>660</v>
+      </c>
+      <c r="L143" t="n">
+        <v>106</v>
+      </c>
+      <c r="M143" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="144">
@@ -5048,7 +7203,22 @@
         </is>
       </c>
       <c r="H144" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I144" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J144" t="n">
+        <v>191</v>
+      </c>
+      <c r="K144" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L144" t="n">
+        <v>264</v>
+      </c>
+      <c r="M144" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="145">
@@ -5080,7 +7250,22 @@
         </is>
       </c>
       <c r="H145" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I145" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J145" t="n">
+        <v>191</v>
+      </c>
+      <c r="K145" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L145" t="n">
+        <v>264</v>
+      </c>
+      <c r="M145" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="146">
@@ -5112,7 +7297,22 @@
         </is>
       </c>
       <c r="H146" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I146" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J146" t="n">
+        <v>191</v>
+      </c>
+      <c r="K146" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L146" t="n">
+        <v>264</v>
+      </c>
+      <c r="M146" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="147">
@@ -5144,7 +7344,22 @@
         </is>
       </c>
       <c r="H147" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I147" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J147" t="n">
+        <v>191</v>
+      </c>
+      <c r="K147" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L147" t="n">
+        <v>264</v>
+      </c>
+      <c r="M147" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="148">
@@ -5176,7 +7391,22 @@
         </is>
       </c>
       <c r="H148" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I148" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J148" t="n">
+        <v>191</v>
+      </c>
+      <c r="K148" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L148" t="n">
+        <v>264</v>
+      </c>
+      <c r="M148" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="149">
@@ -5208,7 +7438,22 @@
         </is>
       </c>
       <c r="H149" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I149" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J149" t="n">
+        <v>191</v>
+      </c>
+      <c r="K149" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L149" t="n">
+        <v>264</v>
+      </c>
+      <c r="M149" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="150">
@@ -5240,7 +7485,22 @@
         </is>
       </c>
       <c r="H150" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I150" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J150" t="n">
+        <v>191</v>
+      </c>
+      <c r="K150" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L150" t="n">
+        <v>264</v>
+      </c>
+      <c r="M150" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="151">
@@ -5272,7 +7532,22 @@
         </is>
       </c>
       <c r="H151" t="n">
-        <v>8</v>
+        <v>10.5555822335</v>
+      </c>
+      <c r="I151" t="n">
+        <v>704.1999999999999</v>
+      </c>
+      <c r="J151" t="n">
+        <v>191</v>
+      </c>
+      <c r="K151" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L151" t="n">
+        <v>264</v>
+      </c>
+      <c r="M151" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="152">
@@ -5304,7 +7579,22 @@
         </is>
       </c>
       <c r="H152" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I152" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J152" t="n">
+        <v>200</v>
+      </c>
+      <c r="K152" t="n">
+        <v>843</v>
+      </c>
+      <c r="L152" t="n">
+        <v>145</v>
+      </c>
+      <c r="M152" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="153">
@@ -5336,7 +7626,22 @@
         </is>
       </c>
       <c r="H153" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I153" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J153" t="n">
+        <v>200</v>
+      </c>
+      <c r="K153" t="n">
+        <v>843</v>
+      </c>
+      <c r="L153" t="n">
+        <v>145</v>
+      </c>
+      <c r="M153" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="154">
@@ -5368,7 +7673,22 @@
         </is>
       </c>
       <c r="H154" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I154" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J154" t="n">
+        <v>200</v>
+      </c>
+      <c r="K154" t="n">
+        <v>843</v>
+      </c>
+      <c r="L154" t="n">
+        <v>145</v>
+      </c>
+      <c r="M154" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="155">
@@ -5400,7 +7720,22 @@
         </is>
       </c>
       <c r="H155" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I155" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J155" t="n">
+        <v>200</v>
+      </c>
+      <c r="K155" t="n">
+        <v>843</v>
+      </c>
+      <c r="L155" t="n">
+        <v>145</v>
+      </c>
+      <c r="M155" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="156">
@@ -5432,7 +7767,22 @@
         </is>
       </c>
       <c r="H156" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I156" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J156" t="n">
+        <v>200</v>
+      </c>
+      <c r="K156" t="n">
+        <v>843</v>
+      </c>
+      <c r="L156" t="n">
+        <v>145</v>
+      </c>
+      <c r="M156" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="157">
@@ -5464,7 +7814,22 @@
         </is>
       </c>
       <c r="H157" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I157" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J157" t="n">
+        <v>200</v>
+      </c>
+      <c r="K157" t="n">
+        <v>843</v>
+      </c>
+      <c r="L157" t="n">
+        <v>145</v>
+      </c>
+      <c r="M157" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="158">
@@ -5496,7 +7861,22 @@
         </is>
       </c>
       <c r="H158" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I158" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J158" t="n">
+        <v>200</v>
+      </c>
+      <c r="K158" t="n">
+        <v>843</v>
+      </c>
+      <c r="L158" t="n">
+        <v>145</v>
+      </c>
+      <c r="M158" t="n">
+        <v>1664.532</v>
       </c>
     </row>
     <row r="159">
@@ -5528,7 +7908,22 @@
         </is>
       </c>
       <c r="H159" t="n">
-        <v>8</v>
+        <v>10.23620925</v>
+      </c>
+      <c r="I159" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="J159" t="n">
+        <v>200</v>
+      </c>
+      <c r="K159" t="n">
+        <v>843</v>
+      </c>
+      <c r="L159" t="n">
+        <v>145</v>
+      </c>
+      <c r="M159" t="n">
+        <v>1664.532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>